<commit_message>
view password loc changed
</commit_message>
<xml_diff>
--- a/Unit Test Plan .xlsx
+++ b/Unit Test Plan .xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setti\Downloads\HiFieats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFD353A-2854-438D-B745-E12F6501E42B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F2CDA4-B89E-409E-8999-A15F14FD0A75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="186">
   <si>
     <t>TEAM 1</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Actual Result</t>
   </si>
   <si>
-    <t>Email validation</t>
-  </si>
-  <si>
     <t>Manual</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>Yes,given invalid email id</t>
   </si>
   <si>
-    <t>Phone number</t>
-  </si>
-  <si>
     <t>exact 10 digits should be there</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t>Yes,given invalid phone number</t>
   </si>
   <si>
-    <t xml:space="preserve">Login page password validation </t>
-  </si>
-  <si>
     <t>username,password should be matched</t>
   </si>
   <si>
@@ -88,9 +79,6 @@
     <t>if condition meets ok,else display required constraints to user</t>
   </si>
   <si>
-    <t>Otp validation</t>
-  </si>
-  <si>
     <t>checking whether otp is receiving to user or not</t>
   </si>
   <si>
@@ -100,99 +88,57 @@
     <t>Yes,it's working</t>
   </si>
   <si>
-    <t>password validation constraints</t>
-  </si>
-  <si>
     <t xml:space="preserve">Password should contain atleast 8 characters long with atleast 1 alphabet, 1 digit ,1 special character included </t>
   </si>
   <si>
     <t>Yes,its showing</t>
   </si>
   <si>
-    <t xml:space="preserve">Password strength display </t>
-  </si>
-  <si>
     <t>Show password strong or weak or moderate to new user</t>
   </si>
   <si>
-    <t xml:space="preserve">mutliple  address of user </t>
-  </si>
-  <si>
     <t>User is able to edit and save or not multiple addresses like home,work,other,etc.</t>
   </si>
   <si>
-    <t>Delivery agent dashboard display view orders</t>
-  </si>
-  <si>
     <t xml:space="preserve">Whether delivery agent is able to view his respective orders </t>
   </si>
   <si>
-    <t xml:space="preserve">Delivery agent performace chart </t>
-  </si>
-  <si>
     <t xml:space="preserve">Should display the performance chart to agent montly based on various parameters like no.of orders, feedback given to him,how fast he is delivering </t>
   </si>
   <si>
-    <t xml:space="preserve">Delivery agent order notifications </t>
-  </si>
-  <si>
     <t>Agent show be notified that a new order has come to deliver</t>
   </si>
   <si>
-    <t>delivery agent issues</t>
-  </si>
-  <si>
     <t>Agent show able to inform admin so that it can be solved</t>
   </si>
   <si>
-    <t>login restrictions</t>
-  </si>
-  <si>
     <t>Backend  and database part should check and restrict them to only one role</t>
   </si>
   <si>
-    <t xml:space="preserve"> delivery agent access </t>
-  </si>
-  <si>
     <t>Admin should update the status so that only delivery agent and customer can login(grant permission and have control over them to access dashboard)</t>
   </si>
   <si>
-    <t>Customer Feedback with Contact Details</t>
-  </si>
-  <si>
     <t>As an admin, they should be able to view customer feedback, including the customer's name and email ID. Access to this information should be restricted to admins only</t>
   </si>
   <si>
-    <t>Item Analysis</t>
-  </si>
-  <si>
     <t>As an admin, they should be able to view the top-selling items in ascending order based on the number of times ordered, allowing the admin to identify the most popular items</t>
   </si>
   <si>
     <t>Admin can views top-selling items in descending order, with the most popular items first.</t>
   </si>
   <si>
-    <t>Customer Order Rating and Review Submission</t>
-  </si>
-  <si>
     <t>As a customer, they should be able to give reviews and ratings only for the food items they have ordered. Additionally: Customers can provide a review and rating only once for the same order and If they have already provided a review, the previous review and rating will be displayed on the same page.</t>
   </si>
   <si>
     <t>Customers can review and rate only ordered items once per order, with their previous review displayed on the same page</t>
   </si>
   <si>
-    <t>Analyze Delivery KPIs</t>
-  </si>
-  <si>
     <t>The system should calculate and display delivery KPIs (e.g., average delivery time, on-time delivery rate) accurately in both graph and table formats based on completed delivery data.</t>
   </si>
   <si>
     <t>Delivery KPIs are displayed accurately in both graph and table formats for performance analysis.</t>
   </si>
   <si>
-    <t xml:space="preserve">Customer Demographics and Order Frequency </t>
-  </si>
-  <si>
     <t>Verify that the customer demographics and order frequency by location are correctly displayed in both a table format and a graph.</t>
   </si>
   <si>
@@ -223,9 +169,6 @@
     <t>Expected Result</t>
   </si>
   <si>
-    <t>Add New Menu Item</t>
-  </si>
-  <si>
     <t>manual testing</t>
   </si>
   <si>
@@ -235,42 +178,24 @@
     <t>Menu item is successfully added.</t>
   </si>
   <si>
-    <t>Add Menu Item with Missing Fields</t>
-  </si>
-  <si>
     <t>Missing required fields (e.g., price).</t>
   </si>
   <si>
-    <t>Add Menu Item with Invalid Price</t>
-  </si>
-  <si>
     <t>Invalid input for price field.</t>
   </si>
   <si>
-    <t>Edit Existing Menu Item</t>
-  </si>
-  <si>
     <t>Valid item ID and updated fields provided.</t>
   </si>
   <si>
-    <t>Edit Menu Item with Invalid Data</t>
-  </si>
-  <si>
     <t>Invalid input for fields during edit.</t>
   </si>
   <si>
-    <t>Delete Existing Menu Item</t>
-  </si>
-  <si>
     <t>Valid item ID provided.</t>
   </si>
   <si>
     <t>Menu item is successfully deleted.</t>
   </si>
   <si>
-    <t>Delete Non-Existent Menu Item</t>
-  </si>
-  <si>
     <t>Invalid menu item ID provided.</t>
   </si>
   <si>
@@ -286,33 +211,18 @@
     <t>No categories available.</t>
   </si>
   <si>
-    <t>Filter Menu Items by Category</t>
-  </si>
-  <si>
     <t>Category filter applied.</t>
   </si>
   <si>
-    <t>Filter Menu Items by Dietary Pref</t>
-  </si>
-  <si>
     <t>Dietary preference filter applied.</t>
   </si>
   <si>
-    <t>Filter with Multiple Conditions</t>
-  </si>
-  <si>
     <t>Both filters applied simultaneously.</t>
   </si>
   <si>
-    <t>Filter with No Results</t>
-  </si>
-  <si>
     <t>Filter conditions yield no results.</t>
   </si>
   <si>
-    <t>Display Menu Item Details</t>
-  </si>
-  <si>
     <t>Menu item data is fetched correctly.</t>
   </si>
   <si>
@@ -328,9 +238,6 @@
     <t>Test procedure</t>
   </si>
   <si>
-    <t>menu displays categories (e.g., Drinks, Desserts, Main Course)</t>
-  </si>
-  <si>
     <t>Ensure categories are dynamically fetched and displayed correctly</t>
   </si>
   <si>
@@ -340,9 +247,6 @@
     <t>Yes, it is showing</t>
   </si>
   <si>
-    <t>clicking on a category displays relevant items</t>
-  </si>
-  <si>
     <t>On selecting the category non-veg/veg the relevant items are being displayed</t>
   </si>
   <si>
@@ -352,9 +256,6 @@
     <t>Yes, it is working</t>
   </si>
   <si>
-    <t>Empty cart should display no items available</t>
-  </si>
-  <si>
     <t>The message display "No items available" in the cart</t>
   </si>
   <si>
@@ -364,75 +265,48 @@
     <t>Yes,it is showing</t>
   </si>
   <si>
-    <t>updating cart counter</t>
-  </si>
-  <si>
     <t>Adding multiple quantities of the same item updates the quantity correctly</t>
   </si>
   <si>
     <t>Allow Adding multiple items</t>
   </si>
   <si>
-    <t>Order tracking</t>
-  </si>
-  <si>
     <t>The order should be tracked from in transit to out for delivery</t>
   </si>
   <si>
     <t>Delivery tracking working</t>
   </si>
   <si>
-    <t>Order Summarization</t>
-  </si>
-  <si>
     <t>Once  you checkout you should be able to see the summary of your order</t>
   </si>
   <si>
     <t>See summary of order</t>
   </si>
   <si>
-    <t>Not showing</t>
-  </si>
-  <si>
-    <t>Delivery location</t>
-  </si>
-  <si>
     <t>If the location of particular order is in range or not and able to edit the location or not</t>
   </si>
   <si>
     <t>Edit Location</t>
   </si>
   <si>
-    <t>Check out without adding items</t>
-  </si>
-  <si>
     <t>If you checkout without adding items in your cart it should display message "YOUR CART IS EMPTY"</t>
   </si>
   <si>
     <t>Show message when empty cart</t>
   </si>
   <si>
-    <t>Cart button,Go to menu</t>
-  </si>
-  <si>
     <t>After selecting items if you go to cart and need to go again to menu there should be a button</t>
   </si>
   <si>
     <t>Go to Menu Button</t>
   </si>
   <si>
-    <t>Increment or decrement items</t>
-  </si>
-  <si>
     <t>You should be able to increment or decrement the items in the cart and the total count should sum up.</t>
   </si>
   <si>
     <t>Total count should show</t>
   </si>
   <si>
-    <t>Place an order and customize it</t>
-  </si>
-  <si>
     <t>Verify that the customer can select items from the menu.</t>
   </si>
   <si>
@@ -442,63 +316,42 @@
     <t>Yes,it is working</t>
   </si>
   <si>
-    <t>Total check</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that the total price updates correctly </t>
   </si>
   <si>
     <t>Total price updates</t>
   </si>
   <si>
-    <t>Order Summary</t>
-  </si>
-  <si>
     <t>Verify that the order with customizations is reflected correctly in the order summary.</t>
   </si>
   <si>
     <t>Customization reflecting</t>
   </si>
   <si>
-    <t>Delivery and pickup options</t>
-  </si>
-  <si>
     <t>Verify that both "Delivery" and "Pickup" options are available during the ordering process</t>
   </si>
   <si>
     <t>Verification</t>
   </si>
   <si>
-    <t>Order Status</t>
-  </si>
-  <si>
     <t>Verify that the order status changes as the order progresses (e.g., Preparing → Out for Delivery → Delivered).</t>
   </si>
   <si>
     <t>Status changes correctly</t>
   </si>
   <si>
-    <t>Past orders</t>
-  </si>
-  <si>
     <t>Verify that a history of past orders is displayed on the customer's account page.</t>
   </si>
   <si>
     <t>past orders displaye for review</t>
   </si>
   <si>
-    <t>Modified orders</t>
-  </si>
-  <si>
     <t>Verify that modified orders update successfully in the system.</t>
   </si>
   <si>
     <t>modified orders update</t>
   </si>
   <si>
-    <t>Special instructions</t>
-  </si>
-  <si>
     <t>Verify that a text field for special instructions is available during checkout.</t>
   </si>
   <si>
@@ -508,36 +361,24 @@
     <t>Not Showing</t>
   </si>
   <si>
-    <t>Orders based on location availability</t>
-  </si>
-  <si>
     <t>Verify that new orders are assigned based on location and availability.</t>
   </si>
   <si>
     <t>new orders assigned</t>
   </si>
   <si>
-    <t>Assign Order to Specific Delivery Person</t>
-  </si>
-  <si>
     <t>Ensure that the restaurant owner can manually assign an order to a specific delivery person.</t>
   </si>
   <si>
     <t>admin must choose delivery agent</t>
   </si>
   <si>
-    <t>View Peak Delivery Times</t>
-  </si>
-  <si>
     <t>Check if the data is grouped correctly by time intervals (e.g., hourly, daily).</t>
   </si>
   <si>
     <t>data grouped</t>
   </si>
   <si>
-    <t>Password constraints</t>
-  </si>
-  <si>
     <t>Error message is displayed .</t>
   </si>
   <si>
@@ -581,6 +422,162 @@
   </si>
   <si>
     <t>SPRINT 3</t>
+  </si>
+  <si>
+    <t>Check Email validation</t>
+  </si>
+  <si>
+    <t>Check Phone Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Login page password validation </t>
+  </si>
+  <si>
+    <t>Check Password constraints</t>
+  </si>
+  <si>
+    <t>Check Otp</t>
+  </si>
+  <si>
+    <t>Check password validation constraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Password strength display </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check mutliple  address of user </t>
+  </si>
+  <si>
+    <t>Check Delivery agent dashboard display view orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Delivery agent performace chart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Delivery agent order notifications </t>
+  </si>
+  <si>
+    <t>Check delivery agent issues</t>
+  </si>
+  <si>
+    <t>Check login restrictions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check delivery agent access </t>
+  </si>
+  <si>
+    <t>Check Customer Feedback with Contact Details</t>
+  </si>
+  <si>
+    <t>Check Item Analysis</t>
+  </si>
+  <si>
+    <t>Check Customer Order Rating and Review Submission</t>
+  </si>
+  <si>
+    <t>Check Analyze Delivery KPIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Customer Demographics and Order Frequency </t>
+  </si>
+  <si>
+    <t>Test Add New Menu Item</t>
+  </si>
+  <si>
+    <t>Test Add Menu Item with Missing Fields</t>
+  </si>
+  <si>
+    <t>Test Add Menu Item with Invalid Price</t>
+  </si>
+  <si>
+    <t>Test Edit Existing Menu Item</t>
+  </si>
+  <si>
+    <t>Test Edit Menu Item with Invalid Data</t>
+  </si>
+  <si>
+    <t>Test Delete Existing Menu Item</t>
+  </si>
+  <si>
+    <t>Test Delete Non-Existent Menu Item</t>
+  </si>
+  <si>
+    <t>Test Filter Menu Items by Category</t>
+  </si>
+  <si>
+    <t>Test Filter Menu Items by Dietary Pref</t>
+  </si>
+  <si>
+    <t>Test Filter with Multiple Conditions</t>
+  </si>
+  <si>
+    <t>Test Filter with No Results</t>
+  </si>
+  <si>
+    <t>Test Display Menu Item Details</t>
+  </si>
+  <si>
+    <t>Test menu displays categories</t>
+  </si>
+  <si>
+    <t>Test clicking on a category displays relevant items</t>
+  </si>
+  <si>
+    <t>Test Empty cart should display no items available</t>
+  </si>
+  <si>
+    <t>Test updating cart counter</t>
+  </si>
+  <si>
+    <t>Test Order tracking</t>
+  </si>
+  <si>
+    <t>Test Order Summarization</t>
+  </si>
+  <si>
+    <t>Test Delivery location</t>
+  </si>
+  <si>
+    <t>Test Check out without adding items</t>
+  </si>
+  <si>
+    <t>Test Cart button,Go to menu</t>
+  </si>
+  <si>
+    <t>Test Increment or decrement items</t>
+  </si>
+  <si>
+    <t>Test Place an order and customize it</t>
+  </si>
+  <si>
+    <t>Test Total check</t>
+  </si>
+  <si>
+    <t>Test Order Summary</t>
+  </si>
+  <si>
+    <t>Test Delivery and pickup options</t>
+  </si>
+  <si>
+    <t>Test Order Status</t>
+  </si>
+  <si>
+    <t>Test Past orders</t>
+  </si>
+  <si>
+    <t>Test Modified orders</t>
+  </si>
+  <si>
+    <t>Test Special instructions</t>
+  </si>
+  <si>
+    <t>Test Orders based on location availability</t>
+  </si>
+  <si>
+    <t>Test Assign Order to Specific Delivery Person</t>
+  </si>
+  <si>
+    <t>Test View Peak Delivery Times</t>
   </si>
 </sst>
 </file>
@@ -1108,6 +1105,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1116,9 +1116,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1604,8 +1601,8 @@
   </sheetPr>
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1618,27 +1615,27 @@
     <col min="6" max="6" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+    </row>
+    <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1646,7 +1643,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1666,107 +1663,107 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>4</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>5</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>22</v>
+        <v>138</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1774,17 +1771,17 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>184</v>
-      </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+    </row>
+    <row r="12" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -1804,187 +1801,187 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>26</v>
+        <v>139</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>2</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>29</v>
+        <v>140</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>3</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>4</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>5</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>6</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>37</v>
+        <v>144</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>7</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>8</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>9</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1992,17 +1989,17 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
-        <v>185</v>
-      </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+    </row>
+    <row r="24" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
@@ -2022,483 +2019,483 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>45</v>
+        <v>148</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>2</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>4</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>5</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>56</v>
+        <v>152</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>6</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
-        <v>183</v>
-      </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+    </row>
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F34" s="22" t="s">
         <v>6</v>
       </c>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>1</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>67</v>
+        <v>153</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="26">
         <v>2</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>71</v>
+        <v>154</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="29">
         <v>3</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>173</v>
+        <v>120</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="26">
         <v>4</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>75</v>
+        <v>156</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>174</v>
+        <v>121</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="29">
         <v>5</v>
       </c>
       <c r="B39" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="F39" s="25" t="s">
-        <v>109</v>
-      </c>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="26">
         <v>6</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
         <v>7</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>176</v>
+        <v>123</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="26">
         <v>8</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>177</v>
+        <v>124</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="29">
         <v>9</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="26">
         <v>10</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>88</v>
+        <v>160</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="29">
         <v>11</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="26">
         <v>12</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>92</v>
+        <v>162</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="29">
         <v>13</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>94</v>
+        <v>163</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>180</v>
+        <v>127</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="26">
         <v>14</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>96</v>
+        <v>164</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="30">
         <v>15</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="E49" s="31" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="F49" s="25" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2507,7 +2504,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2516,7 +2513,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2525,249 +2522,249 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="43" t="s">
-        <v>184</v>
-      </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="43"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
+    <row r="53" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A53" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>1</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="33">
         <v>2</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>106</v>
+        <v>166</v>
       </c>
       <c r="C56" s="34" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="E56" s="34" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="F56" s="35" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>3</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="33">
         <v>4</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D58" s="34" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="E58" s="34" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="F58" s="35" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>5</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>117</v>
+        <v>169</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="33">
         <v>6</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="C60" s="34" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D60" s="34" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="E60" s="34" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="F60" s="35" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>7</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="33">
         <v>8</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="C62" s="34" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="E62" s="34" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="F62" s="35" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>9</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>130</v>
+        <v>173</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="36">
         <v>10</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="E64" s="37" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="F64" s="38" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2776,7 +2773,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2785,7 +2782,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2794,270 +2791,270 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="43" t="s">
-        <v>186</v>
-      </c>
-      <c r="B68" s="43"/>
-      <c r="C68" s="43"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
+    <row r="68" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A68" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>1</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>138</v>
+        <v>96</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="33">
         <v>2</v>
       </c>
       <c r="B71" s="34" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="C71" s="34" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="E71" s="34" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="F71" s="35" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>3</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="33">
         <v>4</v>
       </c>
       <c r="B73" s="34" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="C73" s="34" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D73" s="34" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="E73" s="34" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="F73" s="35" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>5</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="33">
         <v>6</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C75" s="34" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D75" s="34" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="E75" s="34" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
       <c r="F75" s="35" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>7</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="33">
         <v>8</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="C77" s="34" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D77" s="34" t="s">
-        <v>159</v>
+        <v>110</v>
       </c>
       <c r="E77" s="34" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="F77" s="35" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>9</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="33">
         <v>10</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="C79" s="34" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D79" s="34" t="s">
-        <v>166</v>
+        <v>115</v>
       </c>
       <c r="E79" s="34" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="F79" s="35" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <v>11</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>

</xml_diff>

<commit_message>
Updated Test Case Names
</commit_message>
<xml_diff>
--- a/Unit Test Plan .xlsx
+++ b/Unit Test Plan .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setti\Downloads\HiFieats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F2CDA4-B89E-409E-8999-A15F14FD0A75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1002658-8609-42D3-9F61-2FD8C4205C07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,9 +226,6 @@
     <t>Menu item data is fetched correctly.</t>
   </si>
   <si>
-    <t>Handle Missing Images</t>
-  </si>
-  <si>
     <t>Image path is invalid or missing.</t>
   </si>
   <si>
@@ -578,6 +575,9 @@
   </si>
   <si>
     <t>Test View Peak Delivery Times</t>
+  </si>
+  <si>
+    <t>Test how Missing Images are handled</t>
   </si>
 </sst>
 </file>
@@ -1601,8 +1601,8 @@
   </sheetPr>
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1668,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>7</v>
@@ -1688,7 +1688,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>7</v>
@@ -1708,7 +1708,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>7</v>
@@ -1728,7 +1728,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>7</v>
@@ -1748,7 +1748,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>7</v>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="11" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
@@ -1806,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>7</v>
@@ -1826,7 +1826,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>7</v>
@@ -1846,7 +1846,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>7</v>
@@ -1866,7 +1866,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>7</v>
@@ -1886,7 +1886,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>7</v>
@@ -1906,7 +1906,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
@@ -1926,7 +1926,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>7</v>
@@ -1946,7 +1946,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>7</v>
@@ -1966,7 +1966,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>7</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
@@ -2024,7 +2024,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>7</v>
@@ -2044,7 +2044,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>7</v>
@@ -2064,7 +2064,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>7</v>
@@ -2084,7 +2084,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>7</v>
@@ -2104,7 +2104,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>7</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
@@ -2185,7 +2185,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C35" s="24" t="s">
         <v>49</v>
@@ -2197,7 +2197,7 @@
         <v>51</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -2206,7 +2206,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>49</v>
@@ -2215,10 +2215,10 @@
         <v>52</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G36" s="1"/>
     </row>
@@ -2227,7 +2227,7 @@
         <v>3</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C37" s="24" t="s">
         <v>49</v>
@@ -2236,10 +2236,10 @@
         <v>53</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -2248,7 +2248,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>49</v>
@@ -2257,10 +2257,10 @@
         <v>54</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G38" s="1"/>
     </row>
@@ -2269,7 +2269,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>49</v>
@@ -2278,10 +2278,10 @@
         <v>55</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -2290,7 +2290,7 @@
         <v>6</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>49</v>
@@ -2302,7 +2302,7 @@
         <v>57</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -2311,7 +2311,7 @@
         <v>7</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>49</v>
@@ -2320,10 +2320,10 @@
         <v>58</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -2341,10 +2341,10 @@
         <v>60</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -2362,10 +2362,10 @@
         <v>62</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -2374,7 +2374,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C44" s="28" t="s">
         <v>49</v>
@@ -2383,10 +2383,10 @@
         <v>63</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -2395,7 +2395,7 @@
         <v>11</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>49</v>
@@ -2404,10 +2404,10 @@
         <v>64</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G45" s="1"/>
     </row>
@@ -2416,7 +2416,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C46" s="28" t="s">
         <v>49</v>
@@ -2425,10 +2425,10 @@
         <v>65</v>
       </c>
       <c r="E46" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G46" s="1"/>
     </row>
@@ -2437,7 +2437,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>49</v>
@@ -2446,10 +2446,10 @@
         <v>66</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -2458,7 +2458,7 @@
         <v>14</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C48" s="28" t="s">
         <v>49</v>
@@ -2467,10 +2467,10 @@
         <v>67</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -2479,19 +2479,19 @@
         <v>15</v>
       </c>
       <c r="B49" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="31" t="s">
-        <v>69</v>
-      </c>
       <c r="E49" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F49" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="53" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B53" s="39"/>
       <c r="C53" s="39"/>
@@ -2538,10 +2538,10 @@
         <v>45</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>4</v>
@@ -2559,19 +2559,19 @@
         <v>1</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D55" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="F55" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="G55" s="1"/>
     </row>
@@ -2580,19 +2580,19 @@
         <v>2</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C56" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D56" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E56" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="E56" s="34" t="s">
+      <c r="F56" s="35" t="s">
         <v>76</v>
-      </c>
-      <c r="F56" s="35" t="s">
-        <v>77</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -2601,19 +2601,19 @@
         <v>3</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D57" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="F57" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="G57" s="1"/>
     </row>
@@ -2622,19 +2622,19 @@
         <v>4</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C58" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D58" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="E58" s="34" t="s">
-        <v>82</v>
-      </c>
       <c r="F58" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -2643,19 +2643,19 @@
         <v>5</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D59" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="F59" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2664,19 +2664,19 @@
         <v>6</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C60" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D60" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="E60" s="34" t="s">
-        <v>86</v>
-      </c>
       <c r="F60" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2685,19 +2685,19 @@
         <v>7</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D61" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E61" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="F61" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G61" s="1"/>
     </row>
@@ -2706,19 +2706,19 @@
         <v>8</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C62" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D62" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E62" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="E62" s="34" t="s">
-        <v>90</v>
-      </c>
       <c r="F62" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2727,19 +2727,19 @@
         <v>9</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D63" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E63" s="6" t="s">
-        <v>92</v>
-      </c>
       <c r="F63" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G63" s="1"/>
     </row>
@@ -2748,19 +2748,19 @@
         <v>10</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C64" s="37" t="s">
         <v>49</v>
       </c>
       <c r="D64" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="E64" s="37" t="s">
-        <v>94</v>
-      </c>
       <c r="F64" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G64" s="1"/>
     </row>
@@ -2793,7 +2793,7 @@
     </row>
     <row r="68" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
@@ -2807,10 +2807,10 @@
         <v>45</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>4</v>
@@ -2828,19 +2828,19 @@
         <v>1</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D70" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="F70" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="G70" s="1"/>
     </row>
@@ -2849,19 +2849,19 @@
         <v>2</v>
       </c>
       <c r="B71" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C71" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D71" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E71" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E71" s="34" t="s">
-        <v>99</v>
-      </c>
       <c r="F71" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G71" s="1"/>
     </row>
@@ -2870,19 +2870,19 @@
         <v>3</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D72" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E72" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="F72" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G72" s="1"/>
     </row>
@@ -2891,19 +2891,19 @@
         <v>4</v>
       </c>
       <c r="B73" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C73" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D73" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="E73" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="E73" s="34" t="s">
-        <v>103</v>
-      </c>
       <c r="F73" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G73" s="1"/>
     </row>
@@ -2912,19 +2912,19 @@
         <v>5</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D74" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E74" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="F74" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G74" s="1"/>
     </row>
@@ -2933,19 +2933,19 @@
         <v>6</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C75" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D75" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="E75" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="E75" s="34" t="s">
-        <v>107</v>
-      </c>
       <c r="F75" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G75" s="1"/>
     </row>
@@ -2954,19 +2954,19 @@
         <v>7</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D76" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E76" s="6" t="s">
-        <v>109</v>
-      </c>
       <c r="F76" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G76" s="1"/>
     </row>
@@ -2975,19 +2975,19 @@
         <v>8</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C77" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D77" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="E77" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="E77" s="34" t="s">
+      <c r="F77" s="35" t="s">
         <v>111</v>
-      </c>
-      <c r="F77" s="35" t="s">
-        <v>112</v>
       </c>
       <c r="G77" s="1"/>
     </row>
@@ -2996,19 +2996,19 @@
         <v>9</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D78" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E78" s="6" t="s">
-        <v>114</v>
-      </c>
       <c r="F78" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G78" s="1"/>
     </row>
@@ -3017,19 +3017,19 @@
         <v>10</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C79" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D79" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="E79" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="E79" s="34" t="s">
-        <v>116</v>
-      </c>
       <c r="F79" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G79" s="1"/>
     </row>
@@ -3038,19 +3038,19 @@
         <v>11</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D80" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E80" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E80" s="18" t="s">
-        <v>118</v>
-      </c>
       <c r="F80" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G80" s="1"/>
     </row>

</xml_diff>